<commit_message>
compared our results to snake grid results
</commit_message>
<xml_diff>
--- a/results/avg_travel_times_per_algorithm_lucky1.xlsx
+++ b/results/avg_travel_times_per_algorithm_lucky1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/304b24243408c27c/Desktop/projects/Salesforce/SalesForceProject/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{EEC528F9-A1A7-4E01-8BF0-0536D62D146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6590F721-6786-4F87-BA1A-FE09E45CC65D}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{EEC528F9-A1A7-4E01-8BF0-0536D62D146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D8C3580-4BA6-48F4-A530-AF07A1EE9E52}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7C03F1F-8F95-406A-9C6A-7965F216271C}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,6 +476,12 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2">
+        <v>535</v>
+      </c>
+      <c r="C2">
+        <v>5504</v>
+      </c>
       <c r="D2">
         <v>502</v>
       </c>
@@ -504,6 +510,12 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0.34762832999999999</v>
+      </c>
+      <c r="C3">
+        <v>3.5763482780000002</v>
       </c>
       <c r="D3">
         <v>0.32618583499999998</v>

</xml_diff>